<commit_message>
Actualizacion de ph y de excel
</commit_message>
<xml_diff>
--- a/Personajes.xlsx
+++ b/Personajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1093CBF0-95F2-4AAC-955C-6633F647BA4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDA205-95BF-4773-9416-BEDF9E071C61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Nombre</t>
   </si>
@@ -148,14 +148,25 @@
   </si>
   <si>
     <t>Rampo Doyle</t>
+  </si>
+  <si>
+    <t>Milla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -183,8 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +496,7 @@
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,12 +618,136 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>33</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="I2">
+        <v>-1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>-1</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>7</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2">
+        <v>16</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>6</v>
+      </c>
+      <c r="AA2">
+        <v>-1</v>
+      </c>
+      <c r="AB2">
+        <v>7</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>4</v>
+      </c>
+      <c r="AF2">
+        <v>6</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>3</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>4</v>
+      </c>
+      <c r="AK2">
+        <v>7</v>
+      </c>
+      <c r="AL2">
+        <v>3</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>3</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadido la funcion competir
</commit_message>
<xml_diff>
--- a/Personajes.xlsx
+++ b/Personajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDA205-95BF-4773-9416-BEDF9E071C61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0359136A-C94B-4F3A-9F35-32D586652A25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Nombre</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Milla</t>
+  </si>
+  <si>
+    <t>Puntos de vida maximo</t>
   </si>
 </sst>
 </file>
@@ -480,13 +483,13 @@
   <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
@@ -504,117 +507,120 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
       <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>